<commit_message>
Added ability to retrieve the sheet names.
That was too easy.

Signed-off-by: Ika Belerma <ika.belerma@gmail.com>
</commit_message>
<xml_diff>
--- a/robot_tests/excel_files/HelloWorldWorkbook.xlsx
+++ b/robot_tests/excel_files/HelloWorldWorkbook.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13620" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Third Sheet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -393,7 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -412,4 +414,38 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the active sheet of the sample xlsx file.
Signed-off-by: Ika Belerma <ika.belerma@gmail.com>
</commit_message>
<xml_diff>
--- a/robot_tests/excel_files/HelloWorldWorkbook.xlsx
+++ b/robot_tests/excel_files/HelloWorldWorkbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="555" yWindow="555" windowWidth="25035" windowHeight="13620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +68,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -395,11 +400,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -422,7 +427,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -437,9 +442,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>